<commit_message>
Essai fix finalisation posologie 2cd8d477f833d63133b2cab9893927339b59bc85
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/CodeSystem-fr-additional-when-codes.xlsx
+++ b/FinalisationMappingPosologie/ig/CodeSystem-fr-additional-when-codes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-31T09:40:44+00:00</t>
+    <t>2025-01-02T08:06:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t>L'événement se produit après [offset] la toilette / event occurs [offset] after toilette (self grooming/washing)</t>
+  </si>
+  <si>
+    <t>ASK</t>
+  </si>
+  <si>
+    <t>L'événement se produit avant [offset] la collation / event occurs [offset] before snack</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>L'événement se produit lors de la collation / event occurs during snack</t>
+  </si>
+  <si>
+    <t>PSK</t>
+  </si>
+  <si>
+    <t>L'événement se produit après [offset] la collation / event occurs [offset] after snack</t>
   </si>
   <si>
     <t>AMS</t>
@@ -524,7 +542,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -700,6 +718,42 @@
       </c>
       <c r="D14" s="2"/>
     </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix error et warning d85830582cfac01af12a3d87bb67082065d6d902
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/CodeSystem-fr-additional-when-codes.xlsx
+++ b/FinalisationMappingPosologie/ig/CodeSystem-fr-additional-when-codes.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-02T08:46:33+00:00</t>
+    <t>2025-01-02T15:15:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,7 +120,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>13</t>
+    <t>16</t>
   </si>
   <si>
     <t>Level</t>

</xml_diff>